<commit_message>
Correcting lead_lag behavior wrt Pandas
</commit_message>
<xml_diff>
--- a/PSDM/test_LL/test_gac.xlsx
+++ b/PSDM/test_LL/test_gac.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/burkhardt_jonathan_epa_gov/Documents/Profile/Desktop/Git/Water_Treatment_Models/PSDM/test_LL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{1C897B11-7B92-4877-9BBD-BCD1130E9FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D33ED5B8-6BFA-4E7F-8472-F721A5291B73}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{1C897B11-7B92-4877-9BBD-BCD1130E9FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E76E294B-3035-4493-85E6-802F32D5C2F6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="3495" windowWidth="38700" windowHeight="15285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kdata (2)" sheetId="5" r:id="rId1"/>
@@ -323,9 +323,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -363,9 +363,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,26 +398,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -450,26 +433,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -649,9 +615,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -677,7 +643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -706,7 +672,7 @@
         <v>48.39686958951701</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -735,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -764,7 +730,7 @@
         <v>0.80816171603242859</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -793,7 +759,7 @@
         <v>103.6875</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -833,9 +799,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -977,7 +943,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1048,7 +1014,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1119,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1145,7 +1111,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1186,7 +1152,7 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1240,12 +1206,12 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1271,7 +1237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -1288,7 +1254,7 @@
         <v>53</v>
       </c>
       <c r="F2">
-        <v>2.6</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>75</v>
@@ -1300,7 +1266,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1317,7 +1283,7 @@
         <v>0.97</v>
       </c>
       <c r="F3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G3">
         <v>0.98</v>
@@ -1329,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1358,7 +1324,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1387,7 +1353,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1429,12 +1395,12 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1446,7 +1412,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1455,7 +1421,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -1467,7 +1433,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -1476,7 +1442,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -1485,7 +1451,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -1497,7 +1463,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1509,7 +1475,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -1521,7 +1487,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1533,7 +1499,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1545,7 +1511,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -1556,7 +1522,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -1564,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1572,7 +1538,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1580,7 +1546,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1588,7 +1554,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1609,12 +1575,12 @@
       <selection activeCell="A66" sqref="A66:A177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -1628,7 +1594,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1642,7 +1608,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1656,7 +1622,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1670,7 +1636,7 @@
         <v>8.76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1684,7 +1650,7 @@
         <v>6.78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1698,7 +1664,7 @@
         <v>7.16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1712,7 +1678,7 @@
         <v>7.16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1726,7 +1692,7 @@
         <v>7.73</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1740,7 +1706,7 @@
         <v>9.24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1754,7 +1720,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1768,7 +1734,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1782,7 +1748,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1796,7 +1762,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1810,7 +1776,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1824,7 +1790,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1838,7 +1804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1852,7 +1818,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1866,7 +1832,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1880,7 +1846,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1894,7 +1860,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1908,7 +1874,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1922,7 +1888,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1936,7 +1902,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1950,7 +1916,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1964,7 +1930,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1978,7 +1944,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1992,7 +1958,7 @@
         <v>6.32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2006,7 +1972,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -2020,7 +1986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2034,7 +2000,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -2048,7 +2014,7 @@
         <v>6.79</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -2062,7 +2028,7 @@
         <v>6.58</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -2076,7 +2042,7 @@
         <v>7.14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -2090,7 +2056,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -2104,7 +2070,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -2118,7 +2084,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -2132,7 +2098,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -2146,7 +2112,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2160,7 +2126,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -2174,7 +2140,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -2188,7 +2154,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2202,7 +2168,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -2216,7 +2182,7 @@
         <v>6.12</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -2230,7 +2196,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2244,7 +2210,7 @@
         <v>8.58</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -2258,7 +2224,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2272,7 +2238,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2286,7 +2252,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -2300,7 +2266,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2314,7 +2280,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -2328,7 +2294,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -2342,7 +2308,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2356,7 +2322,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2370,7 +2336,7 @@
         <v>9.7200000000000006</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2384,7 +2350,7 @@
         <v>26.3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -2398,7 +2364,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -2412,7 +2378,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -2426,7 +2392,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -2440,7 +2406,7 @@
         <v>46.1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -2454,7 +2420,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -2468,7 +2434,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -2482,7 +2448,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -2496,7 +2462,7 @@
         <v>82.3</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -2510,7 +2476,7 @@
         <v>45.1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>53</v>
       </c>
@@ -2524,7 +2490,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -2538,7 +2504,7 @@
         <v>6.03</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>51</v>
       </c>
@@ -2552,7 +2518,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>51</v>
       </c>
@@ -2566,7 +2532,7 @@
         <v>7.61</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -2580,7 +2546,7 @@
         <v>9.19</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -2594,7 +2560,7 @@
         <v>7.77</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>51</v>
       </c>
@@ -2608,7 +2574,7 @@
         <v>6.64</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>51</v>
       </c>
@@ -2622,7 +2588,7 @@
         <v>7.18</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>51</v>
       </c>
@@ -2636,7 +2602,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>51</v>
       </c>
@@ -2650,7 +2616,7 @@
         <v>4.93</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>51</v>
       </c>
@@ -2664,7 +2630,7 @@
         <v>9.1199999999999992</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>51</v>
       </c>
@@ -2678,7 +2644,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>51</v>
       </c>
@@ -2692,7 +2658,7 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>51</v>
       </c>
@@ -2706,7 +2672,7 @@
         <v>8.26</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>51</v>
       </c>
@@ -2720,7 +2686,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>51</v>
       </c>
@@ -2734,7 +2700,7 @@
         <v>8.01</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>51</v>
       </c>
@@ -2748,7 +2714,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>51</v>
       </c>
@@ -2762,7 +2728,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>51</v>
       </c>
@@ -2776,7 +2742,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>51</v>
       </c>
@@ -2790,7 +2756,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>51</v>
       </c>
@@ -2804,7 +2770,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>51</v>
       </c>
@@ -2818,7 +2784,7 @@
         <v>30.3</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>51</v>
       </c>
@@ -2832,7 +2798,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>51</v>
       </c>
@@ -2846,7 +2812,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>51</v>
       </c>
@@ -2860,7 +2826,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>51</v>
       </c>
@@ -2874,7 +2840,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>51</v>
       </c>
@@ -2888,7 +2854,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>51</v>
       </c>
@@ -2902,7 +2868,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>51</v>
       </c>
@@ -2916,7 +2882,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>51</v>
       </c>
@@ -2930,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>51</v>
       </c>
@@ -2944,7 +2910,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>51</v>
       </c>
@@ -2958,7 +2924,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>51</v>
       </c>
@@ -2972,7 +2938,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>51</v>
       </c>
@@ -2986,7 +2952,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>51</v>
       </c>
@@ -3000,7 +2966,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>51</v>
       </c>
@@ -3014,7 +2980,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>51</v>
       </c>
@@ -3028,7 +2994,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -3042,7 +3008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>51</v>
       </c>
@@ -3056,7 +3022,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>51</v>
       </c>
@@ -3070,7 +3036,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>51</v>
       </c>
@@ -3084,7 +3050,7 @@
         <v>9.3800000000000008</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>51</v>
       </c>
@@ -3098,7 +3064,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>51</v>
       </c>
@@ -3112,7 +3078,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>51</v>
       </c>
@@ -3126,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>51</v>
       </c>
@@ -3140,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>51</v>
       </c>
@@ -3154,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>51</v>
       </c>
@@ -3168,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>51</v>
       </c>
@@ -3182,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>51</v>
       </c>
@@ -3196,7 +3162,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>51</v>
       </c>
@@ -3210,7 +3176,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>51</v>
       </c>
@@ -3224,7 +3190,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>51</v>
       </c>
@@ -3238,7 +3204,7 @@
         <v>6.26</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>51</v>
       </c>
@@ -3252,7 +3218,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>51</v>
       </c>
@@ -3266,7 +3232,7 @@
         <v>5.34</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>51</v>
       </c>
@@ -3280,7 +3246,7 @@
         <v>5.34</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>51</v>
       </c>
@@ -3294,7 +3260,7 @@
         <v>6.22</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>51</v>
       </c>
@@ -3308,7 +3274,7 @@
         <v>5.37</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>51</v>
       </c>
@@ -3322,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>51</v>
       </c>
@@ -3336,7 +3302,7 @@
         <v>8.76</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>51</v>
       </c>
@@ -3350,7 +3316,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>51</v>
       </c>
@@ -3364,7 +3330,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>51</v>
       </c>
@@ -3378,7 +3344,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -3392,7 +3358,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -3406,7 +3372,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -3420,7 +3386,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -3434,7 +3400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -3448,7 +3414,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>51</v>
       </c>
@@ -3462,7 +3428,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>51</v>
       </c>
@@ -3476,7 +3442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>51</v>
       </c>
@@ -3490,7 +3456,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>51</v>
       </c>
@@ -3504,7 +3470,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>51</v>
       </c>
@@ -3518,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>51</v>
       </c>
@@ -3532,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>51</v>
       </c>
@@ -3546,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>51</v>
       </c>
@@ -3560,7 +3526,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>51</v>
       </c>
@@ -3574,7 +3540,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>51</v>
       </c>
@@ -3588,7 +3554,7 @@
         <v>5.57</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>51</v>
       </c>
@@ -3602,7 +3568,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>51</v>
       </c>
@@ -3616,7 +3582,7 @@
         <v>9.7799999999999994</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>51</v>
       </c>
@@ -3630,7 +3596,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>51</v>
       </c>
@@ -3644,7 +3610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>51</v>
       </c>
@@ -3658,7 +3624,7 @@
         <v>6.93</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>51</v>
       </c>
@@ -3672,7 +3638,7 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>51</v>
       </c>
@@ -3686,7 +3652,7 @@
         <v>8.49</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>51</v>
       </c>
@@ -3700,7 +3666,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>51</v>
       </c>
@@ -3714,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>51</v>
       </c>
@@ -3728,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>51</v>
       </c>
@@ -3742,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>51</v>
       </c>
@@ -3756,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>51</v>
       </c>
@@ -3770,7 +3736,7 @@
         <v>5.94</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>51</v>
       </c>
@@ -3784,7 +3750,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>51</v>
       </c>
@@ -3798,7 +3764,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>51</v>
       </c>
@@ -3812,7 +3778,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>51</v>
       </c>
@@ -3826,7 +3792,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>51</v>
       </c>
@@ -3840,7 +3806,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>51</v>
       </c>
@@ -3854,7 +3820,7 @@
         <v>9.27</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>51</v>
       </c>
@@ -3868,7 +3834,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>51</v>
       </c>
@@ -3882,7 +3848,7 @@
         <v>8.06</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>51</v>
       </c>
@@ -3896,7 +3862,7 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>51</v>
       </c>
@@ -3910,7 +3876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>51</v>
       </c>
@@ -3924,7 +3890,7 @@
         <v>7.58</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>51</v>
       </c>
@@ -3938,7 +3904,7 @@
         <v>9.32</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>51</v>
       </c>
@@ -3952,7 +3918,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>51</v>
       </c>
@@ -3966,7 +3932,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>51</v>
       </c>
@@ -3980,7 +3946,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>51</v>
       </c>
@@ -3994,7 +3960,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>51</v>
       </c>
@@ -4008,7 +3974,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>51</v>
       </c>
@@ -4022,7 +3988,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>51</v>
       </c>
@@ -4036,7 +4002,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>51</v>
       </c>
@@ -4050,7 +4016,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>51</v>
       </c>
@@ -4064,7 +4030,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>51</v>
       </c>
@@ -4078,7 +4044,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>51</v>
       </c>

</xml_diff>